<commit_message>
fixed error with mgt_rx and mgt_tx interface names hardcoded
</commit_message>
<xml_diff>
--- a/examples/apex_USp/src/apex_ku15p_root.xlsx
+++ b/examples/apex_USp/src/apex_ku15p_root.xlsx
@@ -32,7 +32,7 @@
     <t xml:space="preserve">// file</t>
   </si>
   <si>
-    <t xml:space="preserve">apex_ku15p_root.tab</t>
+    <t xml:space="preserve">apex_ku15p_gty_root.tab</t>
   </si>
   <si>
     <t xml:space="preserve">// columns</t>
@@ -62,7 +62,7 @@
     <t xml:space="preserve">mgt_rx_iface</t>
   </si>
   <si>
-    <t xml:space="preserve">mgt_rx</t>
+    <t xml:space="preserve">mgt_gty_rx</t>
   </si>
   <si>
     <t xml:space="preserve">MGT RX interface name, must match the name indicated in mgt_ports file, interface column</t>
@@ -71,7 +71,7 @@
     <t xml:space="preserve">mgt_tx_iface</t>
   </si>
   <si>
-    <t xml:space="preserve">mgt_tx</t>
+    <t xml:space="preserve">mgt_gty_tx</t>
   </si>
   <si>
     <t xml:space="preserve">MGT TX interface name, must match the name indicated in mgt_ports file, interface column</t>
@@ -80,7 +80,7 @@
     <t xml:space="preserve">phalg_tx_iface</t>
   </si>
   <si>
-    <t xml:space="preserve">phalg_tx</t>
+    <t xml:space="preserve">phalg_gty_tx</t>
   </si>
   <si>
     <t xml:space="preserve">TX phase alignment interface name</t>
@@ -89,7 +89,7 @@
     <t xml:space="preserve">drp_iface</t>
   </si>
   <si>
-    <t xml:space="preserve">drp</t>
+    <t xml:space="preserve">drp_gty</t>
   </si>
   <si>
     <t xml:space="preserve">DRP interface name, must match the name indicated in mgt_ports file, interface column</t>
@@ -98,7 +98,7 @@
     <t xml:space="preserve">interfaces_fname</t>
   </si>
   <si>
-    <t xml:space="preserve">mgt_interfaces.sv</t>
+    <t xml:space="preserve">mgt_gty_interfaces.sv</t>
   </si>
   <si>
     <t xml:space="preserve">name of generated interface file</t>
@@ -107,7 +107,7 @@
     <t xml:space="preserve">mgt_module_fn</t>
   </si>
   <si>
-    <t xml:space="preserve">mgt_module.sv</t>
+    <t xml:space="preserve">mgt_gty_module.sv</t>
   </si>
   <si>
     <t xml:space="preserve">name of generated MGT module file</t>
@@ -116,7 +116,7 @@
     <t xml:space="preserve">common_module_fn</t>
   </si>
   <si>
-    <t xml:space="preserve">common_module.sv</t>
+    <t xml:space="preserve">common_gty_module.sv</t>
   </si>
   <si>
     <t xml:space="preserve">name of generated COMMON module file</t>
@@ -125,7 +125,7 @@
     <t xml:space="preserve">quad_module_fn</t>
   </si>
   <si>
-    <t xml:space="preserve">quad_module.sv</t>
+    <t xml:space="preserve">quad_gty_module.sv</t>
   </si>
   <si>
     <t xml:space="preserve">name of generated QUAD module file</t>
@@ -134,7 +134,7 @@
     <t xml:space="preserve">top_module_name</t>
   </si>
   <si>
-    <t xml:space="preserve">apex_ku15p_serial_io</t>
+    <t xml:space="preserve">apex_ku15p_gty_serial_io</t>
   </si>
   <si>
     <t xml:space="preserve">name of generated top level module. File name will be formed automatically by adding “.sv”</t>
@@ -436,7 +436,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>